<commit_message>
Atualiza propriedades e estrutura do pacote SSIS
As alterações incluem a atualização do `VersionBuild` de 61 para 68 e a modificação do `VersionGUID`. Novas colunas de entrada, como `Name`, `Price` e `Id_Category`, foram adicionadas ao fluxo de dados. Também foram realizadas mudanças na estrutura de layout e nas conexões entre tarefas, melhorando a lógica do fluxo de trabalho. Além disso, um arquivo binário `Produto.xlsx` foi alterado, refletindo diferenças em seu conteúdo.
</commit_message>
<xml_diff>
--- a/Carga/Produto.xlsx
+++ b/Carga/Produto.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmil\OneDrive\Documentos\Material Visual Studio\Vendas E-Commerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://expertiseinteligencia-my.sharepoint.com/personal/yan_sabarense_expertise_net_br/Documents/Documentos/PROJETOS/E-commerce/Carga/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_5E3496156A4ACF1B9001EE42F5C4BDAE119B0935" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7044597C-CF5A-478F-960D-0FA0C68DD050}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="7965"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -180,13 +181,13 @@
     <t>Id_Category</t>
   </si>
   <si>
-    <t>Bolsa Cara</t>
+    <t>Bolsa Caríssima</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,10 +698,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -986,11 +987,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1036,7 @@
         <v>53</v>
       </c>
       <c r="C3">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>